<commit_message>
code function week 10
</commit_message>
<xml_diff>
--- a/Bangbaocaocongviec.xlsx
+++ b/Bangbaocaocongviec.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HieuPhan\Desktop\GitTLCN\pharmacy_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA9B6E37-DA72-40AA-8A17-1D80729BA36D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDB4EE6-E1C8-4F6B-A6C8-0CB3E9B9F4D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Tuần</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>sequence diagram, database diagram, class diagram, giao diện</t>
+  </si>
+  <si>
+    <t>Code chức năng</t>
   </si>
 </sst>
 </file>
@@ -382,7 +385,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B7" sqref="B7:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -451,36 +454,40 @@
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="B7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
@@ -510,9 +517,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="C7:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>